<commit_message>
Updated Testprotocol and Dokumentation
I added some Testing ideas in our Excel
 file, and also finished writing the second day of our Journal
</commit_message>
<xml_diff>
--- a/Dokumentation/PostIt_Testfälle.xlsx
+++ b/Dokumentation/PostIt_Testfälle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Python\Desktop\Dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{958C5A02-ADDF-426C-BFE2-CE891E4B8553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC02F87F-4873-47E0-8800-2A42DAED2288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{9DF1DA7E-D715-49BA-AD95-A9F14AE43B0F}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Bedingung</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Erwartetes Verhalten</t>
   </si>
@@ -55,6 +52,57 @@
   </si>
   <si>
     <t xml:space="preserve">Eigentliches Verhalten </t>
+  </si>
+  <si>
+    <t>Der Code enthält HTML</t>
+  </si>
+  <si>
+    <t>Der Code enthält CSS</t>
+  </si>
+  <si>
+    <t>Der Code enthält Javascript</t>
+  </si>
+  <si>
+    <t>Es hat eine Funktionierende Datenbank</t>
+  </si>
+  <si>
+    <t>Es hat eine Registrationsseite die einen Account erstellt.</t>
+  </si>
+  <si>
+    <t>Es het eine Login Seite.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bei der Registration werden E-Mail adresse und Passwort erfasst. </t>
+  </si>
+  <si>
+    <t>Dabei wird die E-Mail adresse validiert.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beim Login kann man sich mit den korrekten Daten (Passwort und E-Mail adresse) anmelden. </t>
+  </si>
+  <si>
+    <t>Man kann einen Text posten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Der Text wird von andere Benutzer auch gesehen. </t>
+  </si>
+  <si>
+    <t>Es gibt pro Post ein Zeichenlimit von 300 Zeichen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Man kann nur Text posten und keine Bilder, videos, usw. </t>
+  </si>
+  <si>
+    <t>Der Account kann gelöscht werden</t>
+  </si>
+  <si>
+    <t>Das Passwort wird beim eingeben ge-censored damit es sicherer ist</t>
+  </si>
+  <si>
+    <t>Das Passwort kann man  abändern</t>
+  </si>
+  <si>
+    <t>Das Passwort hat bestimmte anforderungen (muss 8 Zeichen lang sein)</t>
   </si>
 </sst>
 </file>
@@ -159,18 +207,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -485,266 +544,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BCBEF5-9024-440B-BA31-AB63D5B9931C}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.90625" customWidth="1"/>
-    <col min="3" max="3" width="27.7265625" customWidth="1"/>
-    <col min="4" max="4" width="24.54296875" customWidth="1"/>
-    <col min="9" max="9" width="5.7265625" customWidth="1"/>
-    <col min="10" max="10" width="22.81640625" customWidth="1"/>
-    <col min="11" max="11" width="27" customWidth="1"/>
-    <col min="12" max="12" width="23.36328125" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="1"/>
+    <col min="2" max="2" width="27.7265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" style="1" customWidth="1"/>
+    <col min="4" max="7" width="10.90625" style="1"/>
+    <col min="8" max="8" width="5.7265625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="22.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.36328125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="2">
+        <v>44711</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6">
-        <v>44711</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="D3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="6">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="6">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="6">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="6">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="6">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>4</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <v>5</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="6">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6">
         <v>9</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="6">
         <v>10</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="6">
         <v>11</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
+      <c r="B14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="6">
         <v>12</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
+      <c r="B15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
         <v>13</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
+      <c r="B16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="6">
         <v>14</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
+      <c r="B17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="6">
         <v>15</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
+      <c r="B18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="6">
         <v>16</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
+      <c r="B19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="6">
         <v>17</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
+      <c r="B20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="6">
         <v>18</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="4">
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="6">
         <v>19</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="4">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="6">
         <v>20</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="6">
         <v>21</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="4">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="6">
         <v>22</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="4">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="6">
         <v>23</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="4">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="6">
         <v>24</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>